<commit_message>
two thirds done with data
</commit_message>
<xml_diff>
--- a/NBA Project/nba-mvp-voting.xlsx
+++ b/NBA Project/nba-mvp-voting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\risha\Desktop\test1\NBA-MVP-Pred\NBA Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FBDBD5-8FD4-4188-9ED0-CC1579DC3085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FA972E-D609-413B-8AEE-22A2F92C82C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="357">
   <si>
     <t>fga</t>
   </si>
@@ -1112,6 +1112,36 @@
   <si>
     <t>6.5</t>
   </si>
+  <si>
+    <t>18.8</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>20.2</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>19.9</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
 </sst>
 </file>
 
@@ -2129,9 +2159,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC662"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="58" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A631" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J645" sqref="J645"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="67" zoomScaleNormal="58" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I630" sqref="I630"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -55731,6 +55761,27 @@
       <c r="A647">
         <v>645</v>
       </c>
+      <c r="B647" t="s">
+        <v>347</v>
+      </c>
+      <c r="C647" t="s">
+        <v>345</v>
+      </c>
+      <c r="D647" t="s">
+        <v>348</v>
+      </c>
+      <c r="E647">
+        <v>25.8</v>
+      </c>
+      <c r="F647">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="G647">
+        <v>30.3</v>
+      </c>
+      <c r="H647">
+        <v>5</v>
+      </c>
       <c r="J647" s="3">
         <v>0</v>
       </c>
@@ -55790,6 +55841,27 @@
       <c r="A648">
         <v>646</v>
       </c>
+      <c r="B648" t="s">
+        <v>349</v>
+      </c>
+      <c r="C648" t="s">
+        <v>350</v>
+      </c>
+      <c r="D648" t="s">
+        <v>351</v>
+      </c>
+      <c r="E648">
+        <v>21.1</v>
+      </c>
+      <c r="F648">
+        <v>0.501</v>
+      </c>
+      <c r="G648">
+        <v>30.9</v>
+      </c>
+      <c r="H648">
+        <v>6.5</v>
+      </c>
       <c r="J648" s="4">
         <v>0</v>
       </c>
@@ -55849,6 +55921,27 @@
       <c r="A649">
         <v>647</v>
       </c>
+      <c r="B649" t="s">
+        <v>352</v>
+      </c>
+      <c r="C649" t="s">
+        <v>353</v>
+      </c>
+      <c r="D649" t="s">
+        <v>340</v>
+      </c>
+      <c r="E649">
+        <v>24.6</v>
+      </c>
+      <c r="F649">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="G649">
+        <v>17.8</v>
+      </c>
+      <c r="H649">
+        <v>7</v>
+      </c>
       <c r="J649" s="3">
         <v>0</v>
       </c>
@@ -55905,6 +55998,27 @@
     <row r="650" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A650">
         <v>648</v>
+      </c>
+      <c r="B650" t="s">
+        <v>354</v>
+      </c>
+      <c r="C650" t="s">
+        <v>355</v>
+      </c>
+      <c r="D650" t="s">
+        <v>356</v>
+      </c>
+      <c r="E650">
+        <v>25.6</v>
+      </c>
+      <c r="F650">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="G650">
+        <v>31.6</v>
+      </c>
+      <c r="H650">
+        <v>8.1</v>
       </c>
       <c r="J650" s="4">
         <v>0</v>

</xml_diff>